<commit_message>
Group saved to excel
</commit_message>
<xml_diff>
--- a/pandas_text.xlsx
+++ b/pandas_text.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="67">
   <si>
     <t>Cibo &amp; Bevande</t>
   </si>
@@ -170,6 +170,51 @@
   </si>
   <si>
     <t>Adjust balance</t>
+  </si>
+  <si>
+    <t>Redditi</t>
+  </si>
+  <si>
+    <t>Income</t>
+  </si>
+  <si>
+    <t>Essenziali_Dovute</t>
+  </si>
+  <si>
+    <t>Bollette_Manutenzione</t>
+  </si>
+  <si>
+    <t>Macchina</t>
+  </si>
+  <si>
+    <t>Salute_Beneficienza</t>
+  </si>
+  <si>
+    <t>Indispensabili_Necessità</t>
+  </si>
+  <si>
+    <t>Spesa_Caffe_Lunch</t>
+  </si>
+  <si>
+    <t>Future</t>
+  </si>
+  <si>
+    <t>Volute_NonEssenziali</t>
+  </si>
+  <si>
+    <t>Selfcare(Clothes &amp; Sport)</t>
+  </si>
+  <si>
+    <t>Fun &amp; Hobbies</t>
+  </si>
+  <si>
+    <t>Travel &amp; Events</t>
+  </si>
+  <si>
+    <t>Nulle_to_del</t>
+  </si>
+  <si>
+    <t>Da cancellare</t>
   </si>
 </sst>
 </file>
@@ -504,14 +549,14 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B57"/>
+  <dimension ref="A1:B119"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="2"/>
   <cols>
-    <col min="1" max="1" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" collapsed="1">
@@ -519,7 +564,7 @@
         <v>0</v>
       </c>
       <c r="B1">
-        <v>-703.6400000000001</v>
+        <v>-240.35</v>
       </c>
     </row>
     <row r="2" spans="1:2" hidden="1" outlineLevel="1">
@@ -527,7 +572,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>-136.3</v>
+        <v>-14.1</v>
       </c>
     </row>
     <row r="3" spans="1:2" hidden="1" outlineLevel="1">
@@ -535,7 +580,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>-38</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:2" hidden="1" outlineLevel="1">
@@ -543,7 +588,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>-529.34</v>
+        <v>-226.25</v>
       </c>
     </row>
     <row r="5" spans="1:2" collapsed="1">
@@ -551,7 +596,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>-1027.59</v>
+        <v>-77.23</v>
       </c>
     </row>
     <row r="6" spans="1:2" hidden="1" outlineLevel="1">
@@ -559,7 +604,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>-565.1800000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:2" hidden="1" outlineLevel="1">
@@ -567,7 +612,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>-299</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:2" hidden="1" outlineLevel="1">
@@ -575,7 +620,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>-163.41</v>
+        <v>-77.23</v>
       </c>
     </row>
     <row r="9" spans="1:2" collapsed="1">
@@ -583,7 +628,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>-1640.84</v>
+        <v>-15.28</v>
       </c>
     </row>
     <row r="10" spans="1:2" hidden="1" outlineLevel="1">
@@ -591,7 +636,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>-625</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:2" hidden="1" outlineLevel="1">
@@ -599,7 +644,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>-650.9399999999999</v>
+        <v>-15.28</v>
       </c>
     </row>
     <row r="12" spans="1:2" hidden="1" outlineLevel="1">
@@ -615,7 +660,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>-364.9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:2" collapsed="1">
@@ -623,7 +668,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>-3.4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:2" hidden="1" outlineLevel="1">
@@ -631,7 +676,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>-3.4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:2" collapsed="1">
@@ -639,7 +684,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>-542.01</v>
+        <v>-193.58</v>
       </c>
     </row>
     <row r="17" spans="1:2" hidden="1" outlineLevel="1">
@@ -655,7 +700,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>-398.63</v>
+        <v>-168.58</v>
       </c>
     </row>
     <row r="19" spans="1:2" hidden="1" outlineLevel="1">
@@ -663,7 +708,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>-114.58</v>
+        <v>-25</v>
       </c>
     </row>
     <row r="20" spans="1:2" hidden="1" outlineLevel="1">
@@ -671,7 +716,7 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>-28.8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:2" collapsed="1">
@@ -679,7 +724,7 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>-2530.61</v>
+        <v>-566.65</v>
       </c>
     </row>
     <row r="22" spans="1:2" hidden="1" outlineLevel="1">
@@ -695,7 +740,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>-846.52</v>
+        <v>-394.65</v>
       </c>
     </row>
     <row r="24" spans="1:2" hidden="1" outlineLevel="1">
@@ -703,7 +748,7 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>-200</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:2" hidden="1" outlineLevel="1">
@@ -711,7 +756,7 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>-43</v>
+        <v>-22</v>
       </c>
     </row>
     <row r="26" spans="1:2" hidden="1" outlineLevel="1">
@@ -719,7 +764,7 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>-74.52</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:2" hidden="1" outlineLevel="1">
@@ -727,7 +772,7 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>-600</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:2" hidden="1" outlineLevel="1">
@@ -735,7 +780,7 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>-616.5700000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:2" collapsed="1">
@@ -743,7 +788,7 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>-1216.57</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:2" hidden="1" outlineLevel="1">
@@ -751,7 +796,7 @@
         <v>26</v>
       </c>
       <c r="B30">
-        <v>-600</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:2" hidden="1" outlineLevel="1">
@@ -759,7 +804,7 @@
         <v>27</v>
       </c>
       <c r="B31">
-        <v>-616.5700000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:2" collapsed="1">
@@ -767,7 +812,7 @@
         <v>29</v>
       </c>
       <c r="B32">
-        <v>-102.95</v>
+        <v>-34.8</v>
       </c>
     </row>
     <row r="33" spans="1:2" hidden="1" outlineLevel="1">
@@ -775,7 +820,7 @@
         <v>30</v>
       </c>
       <c r="B33">
-        <v>-80</v>
+        <v>-20</v>
       </c>
     </row>
     <row r="34" spans="1:2" hidden="1" outlineLevel="1">
@@ -783,7 +828,7 @@
         <v>31</v>
       </c>
       <c r="B34">
-        <v>-22.95</v>
+        <v>-14.8</v>
       </c>
     </row>
     <row r="35" spans="1:2" collapsed="1">
@@ -791,7 +836,7 @@
         <v>32</v>
       </c>
       <c r="B35">
-        <v>-2025</v>
+        <v>-2000</v>
       </c>
     </row>
     <row r="36" spans="1:2" hidden="1" outlineLevel="1">
@@ -831,7 +876,7 @@
         <v>37</v>
       </c>
       <c r="B40">
-        <v>-25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:2" collapsed="1">
@@ -839,7 +884,7 @@
         <v>38</v>
       </c>
       <c r="B41">
-        <v>25</v>
+        <v>22281.77</v>
       </c>
     </row>
     <row r="42" spans="1:2" hidden="1" outlineLevel="1">
@@ -863,7 +908,7 @@
         <v>41</v>
       </c>
       <c r="B44">
-        <v>25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:2" hidden="1" outlineLevel="1">
@@ -871,7 +916,7 @@
         <v>42</v>
       </c>
       <c r="B45">
-        <v>0</v>
+        <v>22281.77</v>
       </c>
     </row>
     <row r="46" spans="1:2" collapsed="1">
@@ -879,7 +924,7 @@
         <v>43</v>
       </c>
       <c r="B46">
-        <v>2699.539999999998</v>
+        <v>-28</v>
       </c>
     </row>
     <row r="47" spans="1:2" hidden="1" outlineLevel="1">
@@ -951,7 +996,7 @@
         <v>49</v>
       </c>
       <c r="B55">
-        <v>-1520</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:2" hidden="1" outlineLevel="1">
@@ -959,7 +1004,7 @@
         <v>50</v>
       </c>
       <c r="B56">
-        <v>4309.539999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:2" hidden="1" outlineLevel="1">
@@ -967,7 +1012,463 @@
         <v>51</v>
       </c>
       <c r="B57">
-        <v>-90</v>
+        <v>-28</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" collapsed="1">
+      <c r="A63" t="s">
+        <v>52</v>
+      </c>
+      <c r="B63">
+        <v>22281.77</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" hidden="1" outlineLevel="1">
+      <c r="A64" t="s">
+        <v>53</v>
+      </c>
+      <c r="B64">
+        <v>22281.77</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" hidden="1" outlineLevel="2">
+      <c r="A65" t="s">
+        <v>42</v>
+      </c>
+      <c r="B65">
+        <v>22281.77</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" hidden="1" outlineLevel="2">
+      <c r="A66" t="s">
+        <v>40</v>
+      </c>
+      <c r="B66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" hidden="1" outlineLevel="2">
+      <c r="A67" t="s">
+        <v>41</v>
+      </c>
+      <c r="B67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" collapsed="1">
+      <c r="A68" t="s">
+        <v>54</v>
+      </c>
+      <c r="B68">
+        <v>-75.08</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" hidden="1" outlineLevel="1">
+      <c r="A69" t="s">
+        <v>55</v>
+      </c>
+      <c r="B69">
+        <v>-15.28</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" hidden="1" outlineLevel="2">
+      <c r="A70" t="s">
+        <v>10</v>
+      </c>
+      <c r="B70">
+        <v>-15.28</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" hidden="1" outlineLevel="2">
+      <c r="A71" t="s">
+        <v>12</v>
+      </c>
+      <c r="B71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" hidden="1" outlineLevel="2">
+      <c r="A72" t="s">
+        <v>11</v>
+      </c>
+      <c r="B72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" hidden="1" outlineLevel="2">
+      <c r="A73" t="s">
+        <v>9</v>
+      </c>
+      <c r="B73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" hidden="1" outlineLevel="1">
+      <c r="A74" t="s">
+        <v>56</v>
+      </c>
+      <c r="B74">
+        <v>-25</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" hidden="1" outlineLevel="2">
+      <c r="A75" t="s">
+        <v>16</v>
+      </c>
+      <c r="B75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" hidden="1" outlineLevel="2">
+      <c r="A76" t="s">
+        <v>18</v>
+      </c>
+      <c r="B76">
+        <v>-25</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" hidden="1" outlineLevel="1">
+      <c r="A77" t="s">
+        <v>57</v>
+      </c>
+      <c r="B77">
+        <v>-34.8</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" hidden="1" outlineLevel="2">
+      <c r="A78" t="s">
+        <v>31</v>
+      </c>
+      <c r="B78">
+        <v>-14.8</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" hidden="1" outlineLevel="2">
+      <c r="A79" t="s">
+        <v>30</v>
+      </c>
+      <c r="B79">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" collapsed="1">
+      <c r="A80" t="s">
+        <v>58</v>
+      </c>
+      <c r="B80">
+        <v>-408.93</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" hidden="1" outlineLevel="1">
+      <c r="A81" t="s">
+        <v>59</v>
+      </c>
+      <c r="B81">
+        <v>-240.35</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" hidden="1" outlineLevel="2">
+      <c r="A82" t="s">
+        <v>1</v>
+      </c>
+      <c r="B82">
+        <v>-14.1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" hidden="1" outlineLevel="2">
+      <c r="A83" t="s">
+        <v>2</v>
+      </c>
+      <c r="B83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" hidden="1" outlineLevel="2">
+      <c r="A84" t="s">
+        <v>3</v>
+      </c>
+      <c r="B84">
+        <v>-226.25</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" hidden="1" outlineLevel="1">
+      <c r="A85" t="s">
+        <v>13</v>
+      </c>
+      <c r="B85">
+        <v>-168.58</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" hidden="1" outlineLevel="2">
+      <c r="A86" t="s">
+        <v>14</v>
+      </c>
+      <c r="B86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" hidden="1" outlineLevel="2">
+      <c r="A87" t="s">
+        <v>17</v>
+      </c>
+      <c r="B87">
+        <v>-168.58</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" hidden="1" outlineLevel="2">
+      <c r="A88" t="s">
+        <v>19</v>
+      </c>
+      <c r="B88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" hidden="1" outlineLevel="1">
+      <c r="A89" t="s">
+        <v>60</v>
+      </c>
+      <c r="B89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" hidden="1" outlineLevel="2">
+      <c r="A90" t="s">
+        <v>37</v>
+      </c>
+      <c r="B90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" hidden="1" outlineLevel="2">
+      <c r="A91" t="s">
+        <v>36</v>
+      </c>
+      <c r="B91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" collapsed="1">
+      <c r="A92" t="s">
+        <v>61</v>
+      </c>
+      <c r="B92">
+        <v>-671.88</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" hidden="1" outlineLevel="1">
+      <c r="A93" t="s">
+        <v>62</v>
+      </c>
+      <c r="B93">
+        <v>-99.23</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" hidden="1" outlineLevel="2">
+      <c r="A94" t="s">
+        <v>5</v>
+      </c>
+      <c r="B94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" hidden="1" outlineLevel="2">
+      <c r="A95" t="s">
+        <v>7</v>
+      </c>
+      <c r="B95">
+        <v>-77.23</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" hidden="1" outlineLevel="2">
+      <c r="A96" t="s">
+        <v>24</v>
+      </c>
+      <c r="B96">
+        <v>-22</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" hidden="1" outlineLevel="2">
+      <c r="A97" t="s">
+        <v>25</v>
+      </c>
+      <c r="B97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" hidden="1" outlineLevel="1">
+      <c r="A98" t="s">
+        <v>63</v>
+      </c>
+      <c r="B98">
+        <v>-422.65</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" hidden="1" outlineLevel="2">
+      <c r="A99" t="s">
+        <v>6</v>
+      </c>
+      <c r="B99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" hidden="1" outlineLevel="2">
+      <c r="A100" t="s">
+        <v>22</v>
+      </c>
+      <c r="B100">
+        <v>-394.65</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" hidden="1" outlineLevel="2">
+      <c r="A101" t="s">
+        <v>23</v>
+      </c>
+      <c r="B101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" hidden="1" outlineLevel="2">
+      <c r="A102" t="s">
+        <v>51</v>
+      </c>
+      <c r="B102">
+        <v>-28</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" hidden="1" outlineLevel="2">
+      <c r="A103" t="s">
+        <v>49</v>
+      </c>
+      <c r="B103">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" hidden="1" outlineLevel="1">
+      <c r="A104" t="s">
+        <v>64</v>
+      </c>
+      <c r="B104">
+        <v>-150</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" hidden="1" outlineLevel="2">
+      <c r="A105" t="s">
+        <v>21</v>
+      </c>
+      <c r="B105">
+        <v>-150</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" hidden="1" outlineLevel="2">
+      <c r="A106" t="s">
+        <v>26</v>
+      </c>
+      <c r="B106">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" hidden="1" outlineLevel="2">
+      <c r="A107" t="s">
+        <v>27</v>
+      </c>
+      <c r="B107">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" collapsed="1">
+      <c r="A108" t="s">
+        <v>65</v>
+      </c>
+      <c r="B108">
+        <v>-2000</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" hidden="1" outlineLevel="1">
+      <c r="A109" t="s">
+        <v>66</v>
+      </c>
+      <c r="B109">
+        <v>-2000</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" hidden="1" outlineLevel="2">
+      <c r="A110" t="s">
+        <v>33</v>
+      </c>
+      <c r="B110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" hidden="1" outlineLevel="2">
+      <c r="A111" t="s">
+        <v>44</v>
+      </c>
+      <c r="B111">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" hidden="1" outlineLevel="2">
+      <c r="A112" t="s">
+        <v>48</v>
+      </c>
+      <c r="B112">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" hidden="1" outlineLevel="2">
+      <c r="A113" t="s">
+        <v>47</v>
+      </c>
+      <c r="B113">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" hidden="1" outlineLevel="2">
+      <c r="A114" t="s">
+        <v>46</v>
+      </c>
+      <c r="B114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" hidden="1" outlineLevel="2">
+      <c r="A115" t="s">
+        <v>35</v>
+      </c>
+      <c r="B115">
+        <v>-2000</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" hidden="1" outlineLevel="2">
+      <c r="A116" t="s">
+        <v>39</v>
+      </c>
+      <c r="B116">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" hidden="1" outlineLevel="2">
+      <c r="A117" t="s">
+        <v>45</v>
+      </c>
+      <c r="B117">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" hidden="1" outlineLevel="2">
+      <c r="A118" t="s">
+        <v>34</v>
+      </c>
+      <c r="B118">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" hidden="1" outlineLevel="2">
+      <c r="A119" t="s">
+        <v>50</v>
+      </c>
+      <c r="B119">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>